<commit_message>
updated results for qPCR
</commit_message>
<xml_diff>
--- a/data/EXP_1/exp1_qPCR_results.xlsx
+++ b/data/EXP_1/exp1_qPCR_results.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviacattau/Documents/GitHub/fish541_lab/data/EXP 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviacattau/Documents/GitHub/fish541_lab/data/EXP_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7220CF49-F5CE-F443-9385-0DACBA298725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895D6FD9-1D8F-9641-AE16-137E616E259B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31260" yWindow="-1380" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32700" yWindow="-2660" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cq (quant) summary" sheetId="8" r:id="rId1"/>
     <sheet name="exp1_qPCR_results" sheetId="9" r:id="rId2"/>
-    <sheet name="SYBR" sheetId="1" r:id="rId3"/>
-    <sheet name="Melt Curve" sheetId="3" r:id="rId4"/>
-    <sheet name="Temperature Curve (all data) " sheetId="4" r:id="rId5"/>
-    <sheet name="Melt Curve Summary" sheetId="5" r:id="rId6"/>
-    <sheet name="amplification results" sheetId="6" r:id="rId7"/>
-    <sheet name="quant plate view " sheetId="7" r:id="rId8"/>
-    <sheet name="Run Information" sheetId="2" r:id="rId9"/>
+    <sheet name="HSC70 only" sheetId="10" r:id="rId3"/>
+    <sheet name="SYBR" sheetId="1" r:id="rId4"/>
+    <sheet name="Melt Curve" sheetId="3" r:id="rId5"/>
+    <sheet name="Temperature Curve (all data) " sheetId="4" r:id="rId6"/>
+    <sheet name="Melt Curve Summary" sheetId="5" r:id="rId7"/>
+    <sheet name="amplification results" sheetId="6" r:id="rId8"/>
+    <sheet name="quant plate view " sheetId="7" r:id="rId9"/>
+    <sheet name="Run Information" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2787" uniqueCount="262">
   <si>
     <t>Well</t>
   </si>
@@ -821,6 +822,12 @@
   <si>
     <t>HS</t>
   </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>STDEV</t>
+  </si>
 </sst>
 </file>
 
@@ -933,7 +940,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -973,6 +980,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,7 +1073,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -1256,6 +1269,14 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3696,13 +3717,133 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="23.25" style="11" customWidth="1"/>
+    <col min="2" max="2" width="37" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10" style="11" customWidth="1"/>
+    <col min="4" max="16384" width="10" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="13">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="1" gridLines="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="0" scale="0" pageOrder="overThenDown" orientation="portrait" blackAndWhite="1" useFirstPageNumber="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D366DB0-ADA9-7F47-A64B-307E5A959B55}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12:K21"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="A1:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4348,6 +4489,667 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF893172-54A9-DD44-B9D7-1B0361EFD03C}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="21.25" customWidth="1"/>
+    <col min="4" max="4" width="21.25" customWidth="1"/>
+    <col min="6" max="6" width="16.75" customWidth="1"/>
+    <col min="7" max="7" width="23.75" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="15.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J1" t="s">
+        <v>254</v>
+      </c>
+      <c r="K1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="45">
+        <v>4</v>
+      </c>
+      <c r="B2" s="45">
+        <v>40</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="45">
+        <v>27.265000000000001</v>
+      </c>
+      <c r="E2" s="46">
+        <f>D2-B2</f>
+        <v>-12.734999999999999</v>
+      </c>
+      <c r="F2" s="46">
+        <f>E2-$G$2</f>
+        <v>-3.5284999999999993</v>
+      </c>
+      <c r="G2" s="46">
+        <f>AVERAGE(E2:E11)</f>
+        <v>-9.2065000000000001</v>
+      </c>
+      <c r="H2" s="46">
+        <f>2^-(F2)</f>
+        <v>11.539429540268184</v>
+      </c>
+      <c r="I2" s="46">
+        <f>AVERAGE(H2:H11)</f>
+        <v>6.3585899125617358</v>
+      </c>
+      <c r="J2" s="46">
+        <f>AVERAGE(H12:H21)</f>
+        <v>13.069237839511521</v>
+      </c>
+      <c r="K2" s="45" t="s">
+        <v>218</v>
+      </c>
+      <c r="L2" s="45">
+        <f>STDEV(H2:H11)</f>
+        <v>10.624780653338311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="45">
+        <v>11</v>
+      </c>
+      <c r="B3" s="45">
+        <v>40</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="45">
+        <v>34.085000000000001</v>
+      </c>
+      <c r="E3" s="46">
+        <f>D3-B3</f>
+        <v>-5.9149999999999991</v>
+      </c>
+      <c r="F3" s="46">
+        <f t="shared" ref="F3:F21" si="0">E3-$G$2</f>
+        <v>3.291500000000001</v>
+      </c>
+      <c r="H3" s="46">
+        <f t="shared" ref="H3:H21" si="1">2^-(F3)</f>
+        <v>0.10213151384121981</v>
+      </c>
+      <c r="K3" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="45">
+        <v>2</v>
+      </c>
+      <c r="B4" s="45">
+        <v>40</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" s="45">
+        <v>26.655000000000001</v>
+      </c>
+      <c r="E4" s="46">
+        <f t="shared" ref="E4:E21" si="2">D4-B4</f>
+        <v>-13.344999999999999</v>
+      </c>
+      <c r="F4" s="46">
+        <f t="shared" si="0"/>
+        <v>-4.1384999999999987</v>
+      </c>
+      <c r="H4" s="46">
+        <f t="shared" si="1"/>
+        <v>17.612160601985828</v>
+      </c>
+      <c r="K4" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="45">
+        <v>17</v>
+      </c>
+      <c r="B5" s="45">
+        <v>40</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" s="45">
+        <v>30.035</v>
+      </c>
+      <c r="E5" s="46">
+        <f t="shared" si="2"/>
+        <v>-9.9649999999999999</v>
+      </c>
+      <c r="F5" s="46">
+        <f t="shared" si="0"/>
+        <v>-0.75849999999999973</v>
+      </c>
+      <c r="H5" s="46">
+        <f t="shared" si="1"/>
+        <v>1.6917307823781607</v>
+      </c>
+      <c r="K5" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="45">
+        <v>18</v>
+      </c>
+      <c r="B6" s="45">
+        <v>40</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>248</v>
+      </c>
+      <c r="D6" s="45">
+        <v>33.380000000000003</v>
+      </c>
+      <c r="E6" s="46">
+        <f t="shared" si="2"/>
+        <v>-6.6199999999999974</v>
+      </c>
+      <c r="F6" s="46">
+        <f t="shared" si="0"/>
+        <v>2.5865000000000027</v>
+      </c>
+      <c r="H6" s="46">
+        <f t="shared" si="1"/>
+        <v>0.16648914239674786</v>
+      </c>
+      <c r="K6" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="45">
+        <v>10</v>
+      </c>
+      <c r="B7" s="45">
+        <v>40</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="45">
+        <v>31.375</v>
+      </c>
+      <c r="E7" s="46">
+        <f t="shared" si="2"/>
+        <v>-8.625</v>
+      </c>
+      <c r="F7" s="46">
+        <f t="shared" si="0"/>
+        <v>0.58150000000000013</v>
+      </c>
+      <c r="H7" s="46">
+        <f t="shared" si="1"/>
+        <v>0.66826860331484983</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="45">
+        <v>19</v>
+      </c>
+      <c r="B8" s="45">
+        <v>40</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="45">
+        <v>33.135000000000005</v>
+      </c>
+      <c r="E8" s="46">
+        <f t="shared" si="2"/>
+        <v>-6.8649999999999949</v>
+      </c>
+      <c r="F8" s="46">
+        <f t="shared" si="0"/>
+        <v>2.3415000000000052</v>
+      </c>
+      <c r="H8" s="46">
+        <f t="shared" si="1"/>
+        <v>0.19730507909464923</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="45">
+        <v>16</v>
+      </c>
+      <c r="B9" s="45">
+        <v>40</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="45">
+        <v>33.08</v>
+      </c>
+      <c r="E9" s="46">
+        <f t="shared" si="2"/>
+        <v>-6.9200000000000017</v>
+      </c>
+      <c r="F9" s="46">
+        <f t="shared" si="0"/>
+        <v>2.2864999999999984</v>
+      </c>
+      <c r="H9" s="46">
+        <f t="shared" si="1"/>
+        <v>0.20497217754434296</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="45">
+        <v>7</v>
+      </c>
+      <c r="B10" s="45">
+        <v>40</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="45">
+        <v>33.094999999999999</v>
+      </c>
+      <c r="E10" s="46">
+        <f t="shared" si="2"/>
+        <v>-6.9050000000000011</v>
+      </c>
+      <c r="F10" s="46">
+        <f t="shared" si="0"/>
+        <v>2.301499999999999</v>
+      </c>
+      <c r="H10" s="46">
+        <f t="shared" si="1"/>
+        <v>0.20285207988667855</v>
+      </c>
+      <c r="K10" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="45">
+        <v>6</v>
+      </c>
+      <c r="B11" s="45">
+        <v>40</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="D11" s="45">
+        <v>25.83</v>
+      </c>
+      <c r="E11" s="46">
+        <f t="shared" si="2"/>
+        <v>-14.170000000000002</v>
+      </c>
+      <c r="F11" s="46">
+        <f t="shared" si="0"/>
+        <v>-4.9635000000000016</v>
+      </c>
+      <c r="H11" s="46">
+        <f t="shared" si="1"/>
+        <v>31.200559604906697</v>
+      </c>
+      <c r="K11" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="57">
+        <v>1</v>
+      </c>
+      <c r="B12" s="57">
+        <v>40</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="57">
+        <v>24.73</v>
+      </c>
+      <c r="E12" s="58">
+        <f t="shared" si="2"/>
+        <v>-15.27</v>
+      </c>
+      <c r="F12" s="58">
+        <f t="shared" si="0"/>
+        <v>-6.0634999999999994</v>
+      </c>
+      <c r="H12" s="58">
+        <f t="shared" si="1"/>
+        <v>66.879863601641588</v>
+      </c>
+      <c r="K12" s="57" t="s">
+        <v>259</v>
+      </c>
+      <c r="L12" s="57">
+        <f>STDEV(H12:H21)</f>
+        <v>22.955920170045442</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="57">
+        <v>14</v>
+      </c>
+      <c r="B13" s="57">
+        <v>40</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" s="57">
+        <v>26.134999999999998</v>
+      </c>
+      <c r="E13" s="58">
+        <f t="shared" si="2"/>
+        <v>-13.865000000000002</v>
+      </c>
+      <c r="F13" s="58">
+        <f t="shared" si="0"/>
+        <v>-4.6585000000000019</v>
+      </c>
+      <c r="H13" s="58">
+        <f t="shared" si="1"/>
+        <v>25.255050124115218</v>
+      </c>
+      <c r="K13" s="57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="57">
+        <v>3</v>
+      </c>
+      <c r="B14" s="57">
+        <v>40</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" s="57">
+        <v>25.6</v>
+      </c>
+      <c r="E14" s="58">
+        <f t="shared" si="2"/>
+        <v>-14.399999999999999</v>
+      </c>
+      <c r="F14" s="58">
+        <f t="shared" si="0"/>
+        <v>-5.1934999999999985</v>
+      </c>
+      <c r="H14" s="58">
+        <f t="shared" si="1"/>
+        <v>36.593106740226887</v>
+      </c>
+      <c r="K14" s="57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="57">
+        <v>12</v>
+      </c>
+      <c r="B15" s="57">
+        <v>40</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="D15" s="57">
+        <v>32.445</v>
+      </c>
+      <c r="E15" s="58">
+        <f t="shared" si="2"/>
+        <v>-7.5549999999999997</v>
+      </c>
+      <c r="F15" s="58">
+        <f t="shared" si="0"/>
+        <v>1.6515000000000004</v>
+      </c>
+      <c r="H15" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3183090322087383</v>
+      </c>
+      <c r="K15" s="57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="57">
+        <v>8</v>
+      </c>
+      <c r="B16" s="57">
+        <v>40</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>239</v>
+      </c>
+      <c r="D16" s="57">
+        <v>33.54</v>
+      </c>
+      <c r="E16" s="58">
+        <f t="shared" si="2"/>
+        <v>-6.4600000000000009</v>
+      </c>
+      <c r="F16" s="58">
+        <f t="shared" si="0"/>
+        <v>2.7464999999999993</v>
+      </c>
+      <c r="H16" s="58">
+        <f t="shared" si="1"/>
+        <v>0.14901195648238691</v>
+      </c>
+      <c r="K16" s="57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="57">
+        <v>5</v>
+      </c>
+      <c r="B17" s="57">
+        <v>40</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" s="57">
+        <v>39.36</v>
+      </c>
+      <c r="E17" s="58">
+        <f t="shared" si="2"/>
+        <v>-0.64000000000000057</v>
+      </c>
+      <c r="F17" s="58">
+        <f t="shared" si="0"/>
+        <v>8.5664999999999996</v>
+      </c>
+      <c r="H17" s="58">
+        <f t="shared" si="1"/>
+        <v>2.637706940863984E-3</v>
+      </c>
+      <c r="K17" s="57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="57">
+        <v>9</v>
+      </c>
+      <c r="B18" s="57">
+        <v>40</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="57">
+        <v>31.134999999999998</v>
+      </c>
+      <c r="E18" s="58">
+        <f t="shared" si="2"/>
+        <v>-8.865000000000002</v>
+      </c>
+      <c r="F18" s="58">
+        <f t="shared" si="0"/>
+        <v>0.34149999999999814</v>
+      </c>
+      <c r="H18" s="58">
+        <f t="shared" si="1"/>
+        <v>0.78922031637860068</v>
+      </c>
+      <c r="K18" s="57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="57">
+        <v>20</v>
+      </c>
+      <c r="B19" s="57">
+        <v>40</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" s="57">
+        <v>34.96</v>
+      </c>
+      <c r="E19" s="58">
+        <f t="shared" si="2"/>
+        <v>-5.0399999999999991</v>
+      </c>
+      <c r="F19" s="58">
+        <f t="shared" si="0"/>
+        <v>4.166500000000001</v>
+      </c>
+      <c r="H19" s="58">
+        <f t="shared" si="1"/>
+        <v>5.5687602796329484E-2</v>
+      </c>
+      <c r="K19" s="57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="57">
+        <v>13</v>
+      </c>
+      <c r="B20" s="57">
+        <v>40</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="D20" s="57">
+        <v>33.634999999999998</v>
+      </c>
+      <c r="E20" s="58">
+        <f t="shared" si="2"/>
+        <v>-6.365000000000002</v>
+      </c>
+      <c r="F20" s="58">
+        <f t="shared" si="0"/>
+        <v>2.8414999999999981</v>
+      </c>
+      <c r="H20" s="58">
+        <f t="shared" si="1"/>
+        <v>0.13951575939037528</v>
+      </c>
+      <c r="K20" s="57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="57">
+        <v>15</v>
+      </c>
+      <c r="B21" s="57">
+        <v>40</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>245</v>
+      </c>
+      <c r="D21" s="57">
+        <v>31.765000000000001</v>
+      </c>
+      <c r="E21" s="58">
+        <f t="shared" si="2"/>
+        <v>-8.2349999999999994</v>
+      </c>
+      <c r="F21" s="58">
+        <f t="shared" si="0"/>
+        <v>0.9715000000000007</v>
+      </c>
+      <c r="H21" s="58">
+        <f t="shared" si="1"/>
+        <v>0.50997555493424995</v>
+      </c>
+      <c r="K21" s="57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K97"/>
   <sheetViews>
@@ -7488,7 +8290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8C7505-193B-D94A-BA86-2566509A8D72}">
   <dimension ref="A1:K97"/>
   <sheetViews>
@@ -10618,7 +11420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4249978-B449-4846-AD87-230DBB3053C9}">
   <dimension ref="A1:CS62"/>
   <sheetViews>
@@ -28799,7 +29601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E52352-7E46-7D4C-A3EF-756B131FE2EB}">
   <dimension ref="A1:G97"/>
   <sheetViews>
@@ -30467,7 +31269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B09771E9-B2CE-DE4A-AABA-E139E374A36A}">
   <dimension ref="A1:CS41"/>
   <sheetViews>
@@ -42495,7 +43297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F02A07-C2BD-4E41-BB1F-423BCDDFE9B4}">
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -43328,124 +44130,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="23.25" style="11" customWidth="1"/>
-    <col min="2" max="2" width="37" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="10" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="12"/>
-    </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="13">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="1" gridLines="1"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="0" scale="0" pageOrder="overThenDown" orientation="portrait" blackAndWhite="1" useFirstPageNumber="1"/>
-</worksheet>
 </file>
</xml_diff>